<commit_message>
updated the count for RLE count at GET L2 and L3
</commit_message>
<xml_diff>
--- a/data/GET_L2.count.xlsx
+++ b/data/GET_L2.count.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -388,6 +388,11 @@
           <t>Near Threatened</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -410,6 +415,9 @@
       <c r="F2">
         <v>0</v>
       </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -432,6 +440,9 @@
       <c r="F3">
         <v>3</v>
       </c>
+      <c r="G3">
+        <v>12</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -454,6 +465,9 @@
       <c r="F4">
         <v>0</v>
       </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -476,6 +490,9 @@
       <c r="F5">
         <v>0</v>
       </c>
+      <c r="G5">
+        <v>17</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -497,6 +514,9 @@
       </c>
       <c r="F6">
         <v>0</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added narrative - summary findings
</commit_message>
<xml_diff>
--- a/data/GET_L2.count.xlsx
+++ b/data/GET_L2.count.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -393,6 +393,16 @@
           <t>Total</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Threat_total</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Threat_prc</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -418,6 +428,12 @@
       <c r="G2">
         <v>4</v>
       </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>75</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -443,6 +459,12 @@
       <c r="G3">
         <v>12</v>
       </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+      <c r="I3">
+        <v>50</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -468,6 +490,12 @@
       <c r="G4">
         <v>4</v>
       </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>75</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -493,6 +521,12 @@
       <c r="G5">
         <v>17</v>
       </c>
+      <c r="H5">
+        <v>11</v>
+      </c>
+      <c r="I5">
+        <v>65</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -517,6 +551,12 @@
       </c>
       <c r="G6">
         <v>8</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>